<commit_message>
imrove tests, fixes, refator
</commit_message>
<xml_diff>
--- a/data/files/datetime_courder_slots_example.xlsx
+++ b/data/files/datetime_courder_slots_example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Регион</t>
   </si>
@@ -46,19 +46,25 @@
     <t>10:00-12:00,13:00-17:00</t>
   </si>
   <si>
-    <t>8:00-19:00</t>
-  </si>
-  <si>
-    <t>03.01.2021 / 11:00-14:00, 15:00-17:00; 03.01.2021 / 17:00-19:00</t>
+    <t>08:00-19:00</t>
+  </si>
+  <si>
+    <t>03.01.2021 / 11:00-14:00, 15:00-17:00; 1.09.2021 / 17:00-19:00</t>
   </si>
   <si>
     <t>Голенищево</t>
   </si>
   <si>
-    <t>9:00-17:00</t>
-  </si>
-  <si>
-    <t>08.03.2021 / 07:00-20:00</t>
+    <t>4.4.2021</t>
+  </si>
+  <si>
+    <t>11:00-12:00,14:00-15:00</t>
+  </si>
+  <si>
+    <t>09:00-17:00</t>
+  </si>
+  <si>
+    <t>05.04.2021 / 05:00-23:00</t>
   </si>
   <si>
     <t>Стандартное название региона, может повторяться</t>
@@ -174,7 +180,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: "Ч:М-Ч:М, Ч:М-Ч:М, ..."</t>
+      <t>: "ЧЧ:ММ-ЧЧ:ММ, ЧЧ:ММ-ЧЧ:ММ, ..."</t>
     </r>
   </si>
   <si>
@@ -187,8 +193,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -208,6 +214,42 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -215,13 +257,29 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -238,36 +296,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -278,21 +306,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,6 +319,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -316,29 +344,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,13 +373,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,19 +517,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,103 +529,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,31 +547,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,17 +582,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,11 +615,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,21 +656,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -659,17 +665,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,16 +684,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -699,141 +705,144 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1158,94 +1167,98 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="28.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="32.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="33.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="33.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="37.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="11.8571428571429" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.2857142857143" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.4285714285714" style="2" customWidth="1"/>
+    <col min="4" max="4" width="33.7142857142857" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.2857142857143" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.7142857142857" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="144" customHeight="1" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>